<commit_message>
solved fib with both recursion and for loop
</commit_message>
<xml_diff>
--- a/Week3_0304_1004/1004/fibSolutionIllustratedWithPicture.xlsx
+++ b/Week3_0304_1004/1004/fibSolutionIllustratedWithPicture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaolu\Documents\WeekLeetCodeChanllenges\Week3_0304_1004\1004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02518E04-E486-462E-8D2E-CCFE063A46DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA709B30-5A6D-4506-BC75-7490E4F67EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F22E83A-25B8-411F-A60E-889C954DDA94}"/>
+    <workbookView xWindow="6030" yWindow="3780" windowWidth="28800" windowHeight="15345" xr2:uid="{1F22E83A-25B8-411F-A60E-889C954DDA94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1E8E40-6B58-4767-9BF9-1AE5209A6B6A}">
   <dimension ref="BS1:CU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CH25" sqref="CH25"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BT7" sqref="BT7:BT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>